<commit_message>
Working on date and time picker
</commit_message>
<xml_diff>
--- a/data/test_data_excel.xlsx
+++ b/data/test_data_excel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>text_verify</t>
   </si>
@@ -181,6 +181,24 @@
   </si>
   <si>
     <t>Indigo</t>
+  </si>
+  <si>
+    <t>date-picker</t>
+  </si>
+  <si>
+    <t>019_url_date_picker</t>
+  </si>
+  <si>
+    <t>019_date_picker</t>
+  </si>
+  <si>
+    <t>June 11 2001</t>
+  </si>
+  <si>
+    <t>019_date_and_time_picker</t>
+  </si>
+  <si>
+    <t>October 2 1879</t>
   </si>
 </sst>
 </file>
@@ -520,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -758,6 +776,30 @@
       </c>
       <c r="B25" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>